<commit_message>
emergency contact - excel connect done
</commit_message>
<xml_diff>
--- a/OrangeAutomation/TestData/orange_data.xlsx
+++ b/OrangeAutomation/TestData/orange_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium Session\OrangeAutomation\OrangeAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FC1339-FD5C-4026-A6EB-D278ABFF2FFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ACE9C3-1A4D-4D66-ABB1-07F10E139737}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23AA8ECF-470A-47C9-BB99-567E1EF6E63D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{23AA8ECF-470A-47C9-BB99-567E1EF6E63D}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="AddEmergencyContactTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +59,63 @@
   </si>
   <si>
     <t>bala126</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Home Telephone</t>
+  </si>
+  <si>
+    <t>Mobile Telephone</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>Expected Value</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Deep</t>
+  </si>
+  <si>
+    <t>Sister</t>
+  </si>
+  <si>
+    <t>545454</t>
+  </si>
+  <si>
+    <t>Deep;545454</t>
+  </si>
+  <si>
+    <t>Faha</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>676767</t>
+  </si>
+  <si>
+    <t>6767</t>
+  </si>
+  <si>
+    <t>Faha;6767;6767</t>
+  </si>
+  <si>
+    <t>Faha12</t>
+  </si>
+  <si>
+    <t>Faha12;6767;6767</t>
   </si>
 </sst>
 </file>
@@ -93,8 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615C5472-06FF-41E6-98D9-24112426628A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
@@ -491,4 +550,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330A6791-F592-4C63-AE55-CABADA1AB21A}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>34343</v>
+      </c>
+      <c r="G2" s="1">
+        <v>343434</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>